<commit_message>
working swap month with back up output file
</commit_message>
<xml_diff>
--- a/input_data/ipd_nurse/roster_output_bak.xlsx
+++ b/input_data/ipd_nurse/roster_output_bak.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10110"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkhunlertkit/Work/Bumrungrad/Perplexity/Rostering/roster/input_data/ipd_nurse/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583C8ACA-F75C-4B47-AE08-789ADE95AB15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="49800" windowHeight="27600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="1" r:id="rId1"/>
@@ -13,7 +19,7 @@
     <sheet name="request summary" sheetId="4" r:id="rId4"/>
     <sheet name="denied requests" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -305,8 +311,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,13 +375,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -413,7 +427,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -447,6 +461,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -481,9 +496,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -656,14 +672,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="31" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="3.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -773,7 +810,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -883,7 +920,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -993,7 +1030,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1103,7 +1140,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1213,7 +1250,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1323,7 +1360,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1433,7 +1470,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -1543,7 +1580,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -1653,7 +1690,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -1763,7 +1800,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1873,7 +1910,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1983,7 +2020,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -2093,7 +2130,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -2203,7 +2240,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -2313,7 +2350,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -2423,7 +2460,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -2533,7 +2570,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:36">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -2643,7 +2680,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -2759,14 +2796,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -2855,7 +2892,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>66</v>
       </c>
@@ -2944,7 +2981,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>67</v>
       </c>
@@ -3033,7 +3070,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>68</v>
       </c>
@@ -3122,7 +3159,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
@@ -3217,19 +3254,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>60</v>
       </c>
@@ -3237,7 +3274,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
@@ -3245,7 +3282,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
@@ -3253,7 +3290,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
@@ -3261,7 +3298,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>63</v>
       </c>
@@ -3269,7 +3306,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
@@ -3277,7 +3314,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>62</v>
       </c>
@@ -3285,7 +3322,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>61</v>
       </c>
@@ -3299,14 +3336,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3320,7 +3357,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3337,7 +3374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3354,7 +3391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3371,7 +3408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3388,7 +3425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3405,7 +3442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3422,7 +3459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3439,7 +3476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3456,7 +3493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3473,7 +3510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3490,7 +3527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3507,7 +3544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3524,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3541,7 +3578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3558,7 +3595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3575,7 +3612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -3592,7 +3629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3609,7 +3646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3632,14 +3669,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -3653,7 +3692,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3670,7 +3709,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3687,7 +3726,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3704,7 +3743,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3721,7 +3760,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3738,7 +3777,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>

</xml_diff>